<commit_message>
changed excel spreadsheet path from absolute to relative
</commit_message>
<xml_diff>
--- a/src/main/resources/CurrencyTamplate.xlsx
+++ b/src/main/resources/CurrencyTamplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTC\Documents\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Currency</t>
   </si>
@@ -42,12 +42,22 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>0,9852</t>
+  </si>
+  <si>
+    <t>117,6594</t>
+  </si>
+  <si>
+    <t>105,3540</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +390,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -401,6 +411,9 @@
       <c r="B2">
         <v>840</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -409,6 +422,9 @@
       <c r="B3">
         <v>978</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -416,6 +432,9 @@
       </c>
       <c r="B4">
         <v>643</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>